<commit_message>
Form 20 Code updated
</commit_message>
<xml_diff>
--- a/Config/Extraction_Config.xlsx
+++ b/Config/Extraction_Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BRADSOL123\PycharmProjects\MNS-Srilanka\MNS-Srilanaka\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C54FBDC-2052-47AF-B2CB-B64E7CCD1A9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44DFDFD-613D-484A-94D8-B6CE02CFB81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -619,14 +619,14 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="48.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.42578125" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Form 10 and additional director code updated
</commit_message>
<xml_diff>
--- a/Config/Extraction_Config.xlsx
+++ b/Config/Extraction_Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BRADSOL123\PycharmProjects\MNS-Srilanka\MNS-Srilanaka\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93646EFA-0A7E-40FD-B561-041130352B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2255EC12-5680-4C87-A0CF-AC342D01A186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="79">
   <si>
     <t>Field_Name</t>
   </si>
@@ -259,6 +259,9 @@
   </si>
   <si>
     <t>no_of_shares</t>
+  </si>
+  <si>
+    <t>additional_directors</t>
   </si>
 </sst>
 </file>
@@ -616,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -784,8 +787,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>23</v>
+      <c r="A8" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -800,27 +803,30 @@
         <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>23</v>
+        <v>78</v>
       </c>
       <c r="H8" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>24</v>
+      <c r="A9" t="s">
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
       </c>
       <c r="H9" t="s">
         <v>35</v>
@@ -828,22 +834,19 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H10" t="s">
         <v>35</v>
@@ -851,22 +854,22 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H11" t="s">
         <v>35</v>
@@ -874,59 +877,62 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>72</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C12" t="s">
-        <v>73</v>
+        <v>32</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
+        <v>34</v>
+      </c>
+      <c r="G12" t="s">
+        <v>31</v>
       </c>
       <c r="H12" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>14</v>
+      <c r="A13" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="H13" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="E14" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H14" t="s">
         <v>41</v>
@@ -934,22 +940,19 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="H15" t="s">
         <v>41</v>
@@ -957,19 +960,22 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="G16" t="s">
+        <v>30</v>
       </c>
       <c r="H16" t="s">
         <v>41</v>
@@ -977,128 +983,128 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
-      </c>
-      <c r="G17" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="H17" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
         <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G18" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H18" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E20" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G20" t="s">
         <v>54</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H20" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" t="s">
-        <v>56</v>
-      </c>
-      <c r="H20" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D21" t="s">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H21" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B22" t="s">
         <v>8</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D22" t="s">
         <v>61</v>
       </c>
       <c r="E22" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H22" t="s">
         <v>64</v>
@@ -1106,41 +1112,61 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D23" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E23" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="H23" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D24" t="s">
         <v>68</v>
       </c>
       <c r="E24" t="s">
+        <v>68</v>
+      </c>
+      <c r="H24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" t="s">
         <v>71</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H25" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Srilanka Open AI and Charges Code updated
</commit_message>
<xml_diff>
--- a/Config/Extraction_Config.xlsx
+++ b/Config/Extraction_Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BRADSOL123\PycharmProjects\MNS-Srilanka\MNS-Srilanaka\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2255EC12-5680-4C87-A0CF-AC342D01A186}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AA34BF1-925C-47A1-B242-29A416CD2BF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -180,9 +180,6 @@
     <t>charge_details</t>
   </si>
   <si>
-    <t>deed_number,date_of_deed,name_of_person_entitled_to_charge,amount_secured,short_particulars_of_property_charged,description_field_under_description_of_instrument_creating_or_evidancing_charge</t>
-  </si>
-  <si>
     <t>open_charges_latest_event</t>
   </si>
   <si>
@@ -262,6 +259,9 @@
   </si>
   <si>
     <t>additional_directors</t>
+  </si>
+  <si>
+    <t>deed_number,date_of_deed,name_of_person_entitled_to_charge,amount_secured_along_with_currency,short_particulars_of_property_charged,description_field_under_description_of_instrument_creating_or_evidancing_charge</t>
   </si>
 </sst>
 </file>
@@ -622,7 +622,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +660,7 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -685,19 +685,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>74</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>75</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H3" t="s">
         <v>35</v>
@@ -788,7 +788,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -803,7 +803,7 @@
         <v>22</v>
       </c>
       <c r="G8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="H8" t="s">
         <v>35</v>
@@ -900,19 +900,19 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
         <v>72</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>73</v>
       </c>
       <c r="D13" t="s">
         <v>10</v>
       </c>
       <c r="E13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H13" t="s">
         <v>35</v>
@@ -946,7 +946,7 @@
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D15" t="s">
         <v>26</v>
@@ -1047,7 +1047,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -1055,119 +1055,119 @@
         <v>19</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" t="s">
         <v>51</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="G20" t="s">
         <v>53</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>54</v>
-      </c>
-      <c r="H20" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" t="s">
         <v>56</v>
-      </c>
-      <c r="B21" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" t="s">
-        <v>57</v>
       </c>
       <c r="D21" t="s">
         <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
         <v>59</v>
       </c>
-      <c r="B22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>60</v>
       </c>
-      <c r="D22" t="s">
-        <v>61</v>
-      </c>
       <c r="E22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
         <v>62</v>
       </c>
-      <c r="B23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" t="s">
+        <v>61</v>
+      </c>
+      <c r="H23" t="s">
         <v>63</v>
-      </c>
-      <c r="D23" t="s">
-        <v>61</v>
-      </c>
-      <c r="E23" t="s">
-        <v>62</v>
-      </c>
-      <c r="H23" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
         <v>66</v>
       </c>
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>67</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
+        <v>67</v>
+      </c>
+      <c r="H24" t="s">
         <v>68</v>
-      </c>
-      <c r="E24" t="s">
-        <v>68</v>
-      </c>
-      <c r="H24" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>75</v>
+      </c>
+      <c r="D25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" t="s">
         <v>70</v>
       </c>
-      <c r="B25" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" t="s">
-        <v>76</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="H25" t="s">
         <v>68</v>
-      </c>
-      <c r="E25" t="s">
-        <v>71</v>
-      </c>
-      <c r="H25" t="s">
-        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>